<commit_message>
found error in the calculations of A0 and R and did almost the whole analysis again. also included alice in the plotting file of the cross sections
</commit_message>
<xml_diff>
--- a/final_beam_currents.xlsx
+++ b/final_beam_currents.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d50fdffd1f97c7a6/Dokumenter/Master/Master-project-code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="8_{E46B36DE-7B82-FD4C-8EDD-E5DBD93D0203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B4D2DFC-BEB1-A140-B83A-3725CFF1CCB2}"/>
+  <xr:revisionPtr revIDLastSave="121" documentId="8_{E46B36DE-7B82-FD4C-8EDD-E5DBD93D0203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4CF337B0-41F7-A04D-8503-38C0A4340717}"/>
   <bookViews>
-    <workbookView xWindow="18800" yWindow="0" windowWidth="10000" windowHeight="18000" xr2:uid="{385A2A32-626D-EB42-A6C3-7BEDE1C151D1}"/>
+    <workbookView xWindow="34520" yWindow="8120" windowWidth="16500" windowHeight="17500" xr2:uid="{385A2A32-626D-EB42-A6C3-7BEDE1C151D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>compartment</t>
   </si>
@@ -46,18 +46,27 @@
   <si>
     <t>beam_current_unc</t>
   </si>
+  <si>
+    <t>beam_current_rel_unc_percent</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -80,8 +89,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -97,6 +107,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -396,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27914C80-F806-7B4E-8DA9-E5FDE3A117B6}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -407,9 +421,10 @@
     <col min="1" max="1" width="13.6640625" customWidth="1"/>
     <col min="2" max="2" width="16.83203125" customWidth="1"/>
     <col min="3" max="3" width="21.33203125" customWidth="1"/>
+    <col min="4" max="4" width="28.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -419,115 +434,158 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>125.94</v>
-      </c>
-      <c r="C2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="1">
+        <v>125.55377721648701</v>
+      </c>
+      <c r="C2" s="1">
+        <v>3.5780003475760198</v>
+      </c>
+      <c r="D2">
+        <f>C2/B2*100</f>
+        <v>2.849775153643229</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>129.11000000000001</v>
-      </c>
-      <c r="C3">
-        <v>3.15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>128.254874539013</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3.3444359828675601</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D11" si="0">C3/B3*100</f>
+        <v>2.6076482433034061</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>131.37</v>
-      </c>
-      <c r="C4">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B4" s="1">
+        <v>129.17083557633799</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2.5916990436032998</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>2.0064119211117477</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>113.74</v>
-      </c>
-      <c r="C5">
-        <v>5.05</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B5" s="1">
+        <v>99.941701353105103</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4.9618732714479101</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>4.9647676638173914</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>2.2599999999999998</v>
-      </c>
-      <c r="C6">
-        <v>15.51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="1">
+        <v>91.843997944286201</v>
+      </c>
+      <c r="C6" s="1">
+        <v>13.4341991251938</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>14.627193312450492</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>90.4</v>
-      </c>
-      <c r="C7">
-        <v>2.33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B7" s="1">
+        <v>93.236102903692299</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2.2069238551302601</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>2.3670271347676226</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>90.94</v>
-      </c>
-      <c r="C8">
-        <v>1.91</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="1">
+        <v>93.0394431596212</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1.6507718963685301</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>1.7742710406557543</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>94.83</v>
-      </c>
-      <c r="C9">
-        <v>1.55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="1">
+        <v>96.774830544290495</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1.2384057876038901</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>1.2796775573139492</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10">
-        <v>91.51</v>
-      </c>
-      <c r="C10">
-        <v>2.4500000000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="1">
+        <v>92.472254654613494</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2.64639270243888</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>2.8618234867563599</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11">
-        <v>89.93</v>
-      </c>
-      <c r="C11">
-        <v>2.2000000000000002</v>
+      <c r="B11" s="1">
+        <v>89.663223081343801</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2.4615302282849099</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>2.7453064296515119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>